<commit_message>
bind java form and view collectly
</commit_message>
<xml_diff>
--- a/resources/shift_template.xlsx
+++ b/resources/shift_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Shift" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,12 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>&lt;jt:forEach items="${employees}" var="employee" indexVar="index"&gt;${index + 1}. ${employee.name}</t>
   </si>
   <si>
     <t>&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>始業時間</t>
+  </si>
+  <si>
+    <t>${openingTime}</t>
+  </si>
+  <si>
+    <t>終業時間</t>
+  </si>
+  <si>
+    <t>${closingTime}</t>
   </si>
 </sst>
 </file>
@@ -117,17 +129,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:AF3"/>
+  <dimension ref="A3:AF8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF4" activeCellId="0" sqref="AF4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.94372294372294"/>
-    <col collapsed="false" hidden="false" max="32" min="2" style="0" width="2.99134199134199"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="9.94372294372294"/>
+    <col collapsed="false" hidden="false" max="32" min="2" style="0" width="3.01731601731602"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -136,6 +146,22 @@
       </c>
       <c r="AF3" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>